<commit_message>
Eroare flitz si nu popeler
</commit_message>
<xml_diff>
--- a/Data-IN-OUT/02. Structurare TXT to XLSX/2.structured_extract.xlsx
+++ b/Data-IN-OUT/02. Structurare TXT to XLSX/2.structured_extract.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,7 +568,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>RON</t>
+          <t>LEI</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -580,11 +580,11 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['Intocmire lista cantitati - Pasaj superior peste CF Port Constanţa']</t>
+          <t>['Intocmire lista cantitati - Pasaj superior peste CF Port Constanța']</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>86.25</v>
+        <v>83.75</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -592,10 +592,10 @@
         </is>
       </c>
       <c r="N2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P2" t="n">
         <v>10</v>
@@ -614,86 +614,6 @@
       </c>
       <c r="U2" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <f>HYPERLINK("C:\Users\tymyp\Desktop\Coduri-Cursor\workflow.procesare.ok\App.Simpla\Data-IN-OUT\01. Gemini OCR PDF to TXT\IN\PTSI SI 25342.pdf", "PTSI SI 25342.pdf")</f>
-        <v/>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>PTSI SI 25342_ocr</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>25342</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>July 1, 2024</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>PRODUCTIVITY TECHNOLOGIES SERVICES (PTSI), INC.</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>PHP</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>2992000</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2.671,428.57</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>320571.43</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>['Legion Slim 5-14APH8 (82750043PH) 107,321 43 2146,428 57\nAMD Ryzen™ 9794CHS (807167,407520Hz, 8MB L2710MB L3)\nNMDIWD GeForce RTX 1060 8GB GDDR6, Boost Clock, 2370ΜΗΣ TOP 105W\nAMD SoC Platfonn\n18GG Suidered LPDDR5A-0400\nMemory soldered to systemboard, no slots\n16/38 soldered memory, not upgradable\nITB SSD M 22280 PCIe@ 4 0x4 NVMed', 'Workstation TS P3_Tower_W630_ES_R 121,600 436,70571\nPhilippines\nStandard Image (Prelead)\nWindows 11 Pro 64\nWindows 11 Pro 64 English\nTower 1100W 92% Adapter\n13th Generation Intel® Core™ 19-13900 vPro® Processor (E-cores up to 4.20 GHz P-cores up to 5.20 GHz)', 'Eaton 5A 2200I-NEMA 2200VA 1200W 9.553.57 38.214 29\nSpecs\nGNEMA Universal Socket\nLine Interactive | with AVR\nCircuit Breaker Protection\n2 Years Warranty']</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>91.25</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Unusual date format: July 1, 2024; Could not verify totals calculation</t>
-        </is>
-      </c>
-      <c r="N3" t="n">
-        <v>9</v>
-      </c>
-      <c r="O3" t="n">
-        <v>10</v>
-      </c>
-      <c r="P3" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>8</v>
-      </c>
-      <c r="R3" t="n">
-        <v>9</v>
-      </c>
-      <c r="S3" t="n">
-        <v>8</v>
-      </c>
-      <c r="T3" t="n">
-        <v>10</v>
-      </c>
-      <c r="U3" t="n">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>